<commit_message>
Fix Critical, High, and Medium QA issues: Config errors, CPO inflation, Prod zones, code cleanup, imports, and logging.
</commit_message>
<xml_diff>
--- a/dashboards_v2/CMO_Dashboard_Complete.xlsx
+++ b/dashboards_v2/CMO_Dashboard_Complete.xlsx
@@ -7,12 +7,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="SEGMENT_PULSE" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="INNOVATION_LAB" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="STRATEGY_COCKPIT" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="UPLOAD_READY_MARKETING" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="UPLOAD_READY_INNOVATION" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="CROSS_REFERENCE" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="SEGMENT PULSE" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="INNOVATION LAB" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="STRATEGY COCKPIT" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="UPLOAD READY MARKETING" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="UPLOAD READY INNOVATION" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="CROSS REFERENCE" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -160,11 +160,11 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -328,12 +328,12 @@
           </marker>
           <xVal>
             <numRef>
-              <f>'SEGMENT_PULSE'!$I$4</f>
+              <f>'SEGMENT PULSE'!$I$4</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>'SEGMENT_PULSE'!$J$4</f>
+              <f>'SEGMENT PULSE'!$J$4</f>
             </numRef>
           </yVal>
         </ser>
@@ -362,12 +362,12 @@
           </marker>
           <xVal>
             <numRef>
-              <f>'SEGMENT_PULSE'!$I$5</f>
+              <f>'SEGMENT PULSE'!$I$5</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>'SEGMENT_PULSE'!$J$5</f>
+              <f>'SEGMENT PULSE'!$J$5</f>
             </numRef>
           </yVal>
         </ser>
@@ -464,7 +464,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'SEGMENT_PULSE'!I26</f>
+              <f>'SEGMENT PULSE'!I26</f>
             </strRef>
           </tx>
           <spPr>
@@ -474,12 +474,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'SEGMENT_PULSE'!$H$27:$H$29</f>
+              <f>'SEGMENT PULSE'!$H$27:$H$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'SEGMENT_PULSE'!$I$27:$I$29</f>
+              <f>'SEGMENT PULSE'!$I$27:$I$29</f>
             </numRef>
           </val>
         </ser>
@@ -488,7 +488,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'SEGMENT_PULSE'!J26</f>
+              <f>'SEGMENT PULSE'!J26</f>
             </strRef>
           </tx>
           <spPr>
@@ -498,12 +498,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'SEGMENT_PULSE'!$H$27:$H$29</f>
+              <f>'SEGMENT PULSE'!$H$27:$H$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'SEGMENT_PULSE'!$J$27:$J$29</f>
+              <f>'SEGMENT PULSE'!$J$27:$J$29</f>
             </numRef>
           </val>
         </ser>
@@ -1000,18 +1000,18 @@
       <c r="C5" s="8" t="n">
         <v>8800</v>
       </c>
-      <c r="D5" s="9" t="n">
-        <v>-13.67</v>
-      </c>
-      <c r="E5" s="10" t="n">
+      <c r="D5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9" t="n">
         <v>0</v>
       </c>
       <c r="F5" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G5" s="11" t="inlineStr">
-        <is>
-          <t>CRITICAL: Boost TV for Allocation</t>
+      <c r="G5" s="10" t="inlineStr">
+        <is>
+          <t>OK</t>
         </is>
       </c>
       <c r="H5" s="5" t="inlineStr">
@@ -1038,18 +1038,18 @@
       <c r="C6" s="8" t="n">
         <v>6000</v>
       </c>
-      <c r="D6" s="9" t="n">
-        <v>-12.42</v>
-      </c>
-      <c r="E6" s="10" t="n">
+      <c r="D6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9" t="n">
         <v>0</v>
       </c>
       <c r="F6" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G6" s="11" t="inlineStr">
-        <is>
-          <t>CRITICAL: Boost TV for Allocation</t>
+      <c r="G6" s="10" t="inlineStr">
+        <is>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -1065,10 +1065,10 @@
       <c r="C7" s="8" t="n">
         <v>4900</v>
       </c>
-      <c r="D7" s="9" t="n">
-        <v>-3.739999999999998</v>
-      </c>
-      <c r="E7" s="10" t="n">
+      <c r="D7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9" t="n">
         <v>0</v>
       </c>
       <c r="F7" s="5" t="n">
@@ -1086,7 +1086,7 @@
           <t>East</t>
         </is>
       </c>
-      <c r="B8" s="10" t="n">
+      <c r="B8" s="9" t="n">
         <v>0</v>
       </c>
       <c r="C8" s="8" t="n">
@@ -1095,7 +1095,7 @@
       <c r="D8" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="10" t="n">
+      <c r="E8" s="9" t="n">
         <v>0</v>
       </c>
       <c r="F8" s="5" t="n">
@@ -1113,7 +1113,7 @@
           <t>South</t>
         </is>
       </c>
-      <c r="B9" s="10" t="n">
+      <c r="B9" s="9" t="n">
         <v>0</v>
       </c>
       <c r="C9" s="8" t="n">
@@ -1122,7 +1122,7 @@
       <c r="D9" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="10" t="n">
+      <c r="E9" s="9" t="n">
         <v>0</v>
       </c>
       <c r="F9" s="5" t="n">
@@ -1193,13 +1193,13 @@
       <c r="D14" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E14" s="10" t="n">
+      <c r="E14" s="9" t="n">
         <v>0</v>
       </c>
       <c r="F14" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G14" s="13" t="inlineStr">
+      <c r="G14" s="10" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1220,13 +1220,13 @@
       <c r="D15" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E15" s="10" t="n">
+      <c r="E15" s="9" t="n">
         <v>0</v>
       </c>
       <c r="F15" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G15" s="13" t="inlineStr">
+      <c r="G15" s="10" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1244,16 +1244,16 @@
       <c r="C16" s="8" t="n">
         <v>12600</v>
       </c>
-      <c r="D16" s="9" t="n">
+      <c r="D16" s="13" t="n">
         <v>-3.552713678800501e-15</v>
       </c>
-      <c r="E16" s="10" t="n">
+      <c r="E16" s="9" t="n">
         <v>0</v>
       </c>
       <c r="F16" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G16" s="13" t="inlineStr">
+      <c r="G16" s="10" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1265,7 +1265,7 @@
           <t>East</t>
         </is>
       </c>
-      <c r="B17" s="10" t="n">
+      <c r="B17" s="9" t="n">
         <v>0</v>
       </c>
       <c r="C17" s="8" t="n">
@@ -1274,7 +1274,7 @@
       <c r="D17" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E17" s="10" t="n">
+      <c r="E17" s="9" t="n">
         <v>0</v>
       </c>
       <c r="F17" s="5" t="n">
@@ -1292,7 +1292,7 @@
           <t>South</t>
         </is>
       </c>
-      <c r="B18" s="10" t="n">
+      <c r="B18" s="9" t="n">
         <v>0</v>
       </c>
       <c r="C18" s="8" t="n">
@@ -1301,7 +1301,7 @@
       <c r="D18" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E18" s="10" t="n">
+      <c r="E18" s="9" t="n">
         <v>0</v>
       </c>
       <c r="F18" s="5" t="n">
@@ -2304,11 +2304,11 @@
         </is>
       </c>
       <c r="D6" s="5">
-        <f>STRATEGY_COCKPIT!C9</f>
+        <f>'STRATEGY COCKPIT'!C9</f>
         <v/>
       </c>
       <c r="E6" s="5">
-        <f>STRATEGY_COCKPIT!B10</f>
+        <f>'STRATEGY COCKPIT'!B10</f>
         <v/>
       </c>
       <c r="G6" s="5" t="inlineStr">
@@ -2317,7 +2317,7 @@
         </is>
       </c>
       <c r="H6" s="5">
-        <f>STRATEGY_COCKPIT!D16</f>
+        <f>'STRATEGY COCKPIT'!D16</f>
         <v/>
       </c>
       <c r="J6" s="5" t="inlineStr">
@@ -2331,7 +2331,7 @@
         </is>
       </c>
       <c r="L6" s="5">
-        <f>STRATEGY_COCKPIT!G16</f>
+        <f>'STRATEGY COCKPIT'!G16</f>
         <v/>
       </c>
       <c r="N6" s="5" t="inlineStr">
@@ -2340,11 +2340,11 @@
         </is>
       </c>
       <c r="O6" s="5">
-        <f>STRATEGY_COCKPIT!I16</f>
+        <f>'STRATEGY COCKPIT'!I16</f>
         <v/>
       </c>
       <c r="P6" s="5">
-        <f>STRATEGY_COCKPIT!F16</f>
+        <f>'STRATEGY COCKPIT'!F16</f>
         <v/>
       </c>
     </row>
@@ -2365,11 +2365,11 @@
         </is>
       </c>
       <c r="D7" s="5">
-        <f>STRATEGY_COCKPIT!E16*STRATEGY_COCKPIT!$B$3</f>
+        <f>'STRATEGY COCKPIT'!E16*'STRATEGY COCKPIT'!$B$3</f>
         <v/>
       </c>
       <c r="E7" s="5">
-        <f>STRATEGY_COCKPIT!B10</f>
+        <f>'STRATEGY COCKPIT'!B10</f>
         <v/>
       </c>
       <c r="G7" s="5" t="inlineStr">
@@ -2378,7 +2378,7 @@
         </is>
       </c>
       <c r="H7" s="5">
-        <f>STRATEGY_COCKPIT!D17</f>
+        <f>'STRATEGY COCKPIT'!D17</f>
         <v/>
       </c>
       <c r="J7" s="5" t="inlineStr">
@@ -2392,7 +2392,7 @@
         </is>
       </c>
       <c r="L7" s="5">
-        <f>STRATEGY_COCKPIT!G17</f>
+        <f>'STRATEGY COCKPIT'!G17</f>
         <v/>
       </c>
       <c r="N7" s="5" t="inlineStr">
@@ -2401,11 +2401,11 @@
         </is>
       </c>
       <c r="O7" s="5">
-        <f>STRATEGY_COCKPIT!I17</f>
+        <f>'STRATEGY COCKPIT'!I17</f>
         <v/>
       </c>
       <c r="P7" s="5">
-        <f>STRATEGY_COCKPIT!F17</f>
+        <f>'STRATEGY COCKPIT'!F17</f>
         <v/>
       </c>
     </row>
@@ -2426,11 +2426,11 @@
         </is>
       </c>
       <c r="D8" s="5">
-        <f>STRATEGY_COCKPIT!E17*STRATEGY_COCKPIT!$B$3</f>
+        <f>'STRATEGY COCKPIT'!E17*'STRATEGY COCKPIT'!$B$3</f>
         <v/>
       </c>
       <c r="E8" s="5">
-        <f>STRATEGY_COCKPIT!B10</f>
+        <f>'STRATEGY COCKPIT'!B10</f>
         <v/>
       </c>
       <c r="G8" s="5" t="inlineStr">
@@ -2439,7 +2439,7 @@
         </is>
       </c>
       <c r="H8" s="5">
-        <f>STRATEGY_COCKPIT!D18</f>
+        <f>'STRATEGY COCKPIT'!D18</f>
         <v/>
       </c>
       <c r="J8" s="5" t="inlineStr">
@@ -2453,7 +2453,7 @@
         </is>
       </c>
       <c r="L8" s="5">
-        <f>STRATEGY_COCKPIT!G18</f>
+        <f>'STRATEGY COCKPIT'!G18</f>
         <v/>
       </c>
       <c r="N8" s="5" t="inlineStr">
@@ -2462,11 +2462,11 @@
         </is>
       </c>
       <c r="O8" s="5">
-        <f>STRATEGY_COCKPIT!I18</f>
+        <f>'STRATEGY COCKPIT'!I18</f>
         <v/>
       </c>
       <c r="P8" s="5">
-        <f>STRATEGY_COCKPIT!F18</f>
+        <f>'STRATEGY COCKPIT'!F18</f>
         <v/>
       </c>
     </row>
@@ -2487,11 +2487,11 @@
         </is>
       </c>
       <c r="D9" s="5">
-        <f>STRATEGY_COCKPIT!E18*STRATEGY_COCKPIT!$B$3</f>
+        <f>'STRATEGY COCKPIT'!E18*'STRATEGY COCKPIT'!$B$3</f>
         <v/>
       </c>
       <c r="E9" s="5">
-        <f>STRATEGY_COCKPIT!B10</f>
+        <f>'STRATEGY COCKPIT'!B10</f>
         <v/>
       </c>
       <c r="G9" s="5" t="inlineStr">
@@ -2500,7 +2500,7 @@
         </is>
       </c>
       <c r="H9" s="5">
-        <f>STRATEGY_COCKPIT!D19</f>
+        <f>'STRATEGY COCKPIT'!D19</f>
         <v/>
       </c>
       <c r="J9" s="5" t="inlineStr">
@@ -2514,7 +2514,7 @@
         </is>
       </c>
       <c r="L9" s="5">
-        <f>STRATEGY_COCKPIT!G19</f>
+        <f>'STRATEGY COCKPIT'!G19</f>
         <v/>
       </c>
       <c r="N9" s="5" t="inlineStr">
@@ -2523,11 +2523,11 @@
         </is>
       </c>
       <c r="O9" s="5">
-        <f>STRATEGY_COCKPIT!I19</f>
+        <f>'STRATEGY COCKPIT'!I19</f>
         <v/>
       </c>
       <c r="P9" s="5">
-        <f>STRATEGY_COCKPIT!F19</f>
+        <f>'STRATEGY COCKPIT'!F19</f>
         <v/>
       </c>
     </row>
@@ -2548,11 +2548,11 @@
         </is>
       </c>
       <c r="D10" s="5">
-        <f>STRATEGY_COCKPIT!E19*STRATEGY_COCKPIT!$B$3</f>
+        <f>'STRATEGY COCKPIT'!E19*'STRATEGY COCKPIT'!$B$3</f>
         <v/>
       </c>
       <c r="E10" s="5">
-        <f>STRATEGY_COCKPIT!B10</f>
+        <f>'STRATEGY COCKPIT'!B10</f>
         <v/>
       </c>
       <c r="G10" s="5" t="inlineStr">
@@ -2561,7 +2561,7 @@
         </is>
       </c>
       <c r="H10" s="5">
-        <f>STRATEGY_COCKPIT!D20</f>
+        <f>'STRATEGY COCKPIT'!D20</f>
         <v/>
       </c>
       <c r="J10" s="5" t="inlineStr">
@@ -2575,7 +2575,7 @@
         </is>
       </c>
       <c r="L10" s="5">
-        <f>STRATEGY_COCKPIT!G20</f>
+        <f>'STRATEGY COCKPIT'!G20</f>
         <v/>
       </c>
       <c r="N10" s="5" t="inlineStr">
@@ -2584,11 +2584,11 @@
         </is>
       </c>
       <c r="O10" s="5">
-        <f>STRATEGY_COCKPIT!I20</f>
+        <f>'STRATEGY COCKPIT'!I20</f>
         <v/>
       </c>
       <c r="P10" s="5">
-        <f>STRATEGY_COCKPIT!F20</f>
+        <f>'STRATEGY COCKPIT'!F20</f>
         <v/>
       </c>
     </row>
@@ -2609,11 +2609,11 @@
         </is>
       </c>
       <c r="D11" s="5">
-        <f>STRATEGY_COCKPIT!E20*STRATEGY_COCKPIT!$B$3</f>
+        <f>'STRATEGY COCKPIT'!E20*'STRATEGY COCKPIT'!$B$3</f>
         <v/>
       </c>
       <c r="E11" s="5">
-        <f>STRATEGY_COCKPIT!B10</f>
+        <f>'STRATEGY COCKPIT'!B10</f>
         <v/>
       </c>
     </row>
@@ -2948,7 +2948,7 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2000</t>
         </is>
       </c>
     </row>
@@ -2960,7 +2960,7 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>85.0%</t>
+          <t>75.0%</t>
         </is>
       </c>
     </row>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="B11" s="5" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>Healthy</t>
         </is>
       </c>
     </row>

</xml_diff>